<commit_message>
Changed kcrew logic on upload pages
</commit_message>
<xml_diff>
--- a/formats/roster_format_download.xlsx
+++ b/formats/roster_format_download.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fletch/Desktop/bluffs_getto/formats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F75A234-8DCC-1242-AD54-60F6F3951CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79793C7E-578D-B949-811B-0173DD65F9ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{6EF3D5C6-2AFF-3846-9FE0-C318AF74BB5A}"/>
   </bookViews>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA5CDA4-92DD-C345-8C03-951E3F1F7434}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="247" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="247" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>